<commit_message>
Correction de la liste des tâches
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15435" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M23"/>
 </workbook>
 </file>
 
@@ -51,176 +52,176 @@
     <t>Validé</t>
   </si>
   <si>
-    <t xml:space="preserve">     Dévelopement et test de la classe Salle</t>
-  </si>
-  <si>
     <t>Classe Salle</t>
   </si>
   <si>
     <t>Classe DAO</t>
   </si>
   <si>
-    <t xml:space="preserve">     Dévelopement et test méthode __construct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode __destruct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode annulerReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode aPasseDesReservations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode confirmerReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode creerLesDigicodesManquants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode creerUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode envoyerMdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode estLeCreateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode existeReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode existeUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode getLesReservations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode getLesSalles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode getNiveauUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode getReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode getUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode modifierMdpUser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode supprimerUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode testerDigicodeBatiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode testerDigicodeSalle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test méthode genererUnDigicode</t>
-  </si>
-  <si>
     <t>Jim</t>
   </si>
   <si>
     <t>Classe Outils</t>
   </si>
   <si>
-    <t xml:space="preserve">     Dévelopement et test de la classe Outils</t>
-  </si>
-  <si>
     <t>Classe Reservation</t>
   </si>
   <si>
-    <t xml:space="preserve">     Dévelopement et test de la classe Reservation</t>
-  </si>
-  <si>
     <t>Classe Utilisateur</t>
   </si>
   <si>
-    <t xml:space="preserve">     Dévelopement et test de la classe Utilisateur</t>
-  </si>
-  <si>
     <t>Vues et Contrôleurs</t>
   </si>
   <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlAnnulerReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueAnnulerReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlChangerDeMdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueChangerDeMdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlConfirmerReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueConfirmerReservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlConnecter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueConnecter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlConsulterReservations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueConsulterReservations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlConsulterSalles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueConsulterSalles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlCreerUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueCreerUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlDemanderMdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueDemanderMdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlMenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueMenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlSupprimerUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test VueSupprimerUtilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test CtrlTelechargerApk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Dévelopement et test page index</t>
-  </si>
-  <si>
     <t>Tous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test de la classe Outils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test de la classe Reservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test de la classe Utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test de la classe Salle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode __construct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode annulerReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode __destruct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode aPasseDesReservations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode confirmerReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode creerLesDigicodesManquants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode creerUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode envoyerMdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode estLeCreateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode existeUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode existeReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode genererUnDigicode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode getLesReservations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode getNiveauUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode getLesSalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode getReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode getUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode modifierMdpUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode supprimerUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode testerDigicodeBatiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test méthode testerDigicodeSalle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test page index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlAnnulerReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueAnnulerReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlChangerDeMdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueChangerDeMdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlConfirmerReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueConfirmerReservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlConnecter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueConnecter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlConsulterReservations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueConsulterReservations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlConsulterSalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueConsulterSalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlCreerUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueCreerUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlDemanderMdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueDemanderMdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlMenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueMenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlSupprimerUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test VueSupprimerUtilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Développement et test CtrlTelechargerApk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,10 +334,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -399,7 +400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,9 +432,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,6 +467,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -640,17 +643,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
@@ -662,18 +665,18 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -682,18 +685,18 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="18.75">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -719,14 +722,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -734,7 +737,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7">
@@ -744,14 +747,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -759,7 +762,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7">
@@ -769,14 +772,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -784,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7">
@@ -794,14 +797,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -813,14 +816,14 @@
       <c r="G17" s="7"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -828,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7">
@@ -838,9 +841,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -848,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7">
@@ -858,9 +861,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -872,9 +875,9 @@
       <c r="G22" s="7"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>4</v>
@@ -886,9 +889,9 @@
       <c r="G23" s="7"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -900,9 +903,9 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -910,7 +913,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="7">
@@ -920,9 +923,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -930,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="7">
@@ -940,9 +943,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>4</v>
@@ -954,9 +957,9 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>4</v>
@@ -968,9 +971,9 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>4</v>
@@ -982,9 +985,9 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -992,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="7">
@@ -1002,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="7">
@@ -1022,9 +1025,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1032,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1040,9 +1043,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>4</v>
@@ -1054,9 +1057,9 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1064,7 +1067,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="7">
@@ -1074,9 +1077,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>4</v>
@@ -1088,9 +1091,9 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>4</v>
@@ -1102,9 +1105,9 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>4</v>
@@ -1116,9 +1119,9 @@
       <c r="G37" s="7"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>4</v>
@@ -1130,9 +1133,9 @@
       <c r="G38" s="7"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>4</v>
@@ -1144,9 +1147,9 @@
       <c r="G39" s="7"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1154,7 +1157,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7">
@@ -1164,9 +1167,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="18.75">
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>0</v>
@@ -1190,9 +1193,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
@@ -1200,15 +1203,15 @@
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>4</v>
@@ -1220,9 +1223,9 @@
       <c r="G47" s="7"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>4</v>
@@ -1234,18 +1237,18 @@
       <c r="G48" s="7"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>4</v>
@@ -1257,9 +1260,9 @@
       <c r="G50" s="7"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>4</v>
@@ -1271,18 +1274,18 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="10"/>
+      <c r="G52" s="9"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>4</v>
@@ -1294,9 +1297,9 @@
       <c r="G53" s="7"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>4</v>
@@ -1308,7 +1311,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -1317,9 +1320,9 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -1327,7 +1330,7 @@
         <v>4</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="7">
@@ -1337,9 +1340,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -1347,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="7">
@@ -1357,18 +1360,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="10"/>
+      <c r="G58" s="9"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -1376,7 +1379,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="7">
@@ -1386,9 +1389,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -1396,7 +1399,7 @@
         <v>4</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="7">
@@ -1406,18 +1409,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="10"/>
+      <c r="G61" s="9"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>4</v>
@@ -1429,9 +1432,9 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>4</v>
@@ -1443,18 +1446,18 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -1462,7 +1465,7 @@
         <v>4</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7">
@@ -1472,9 +1475,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -1482,7 +1485,7 @@
         <v>4</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7">
@@ -1492,18 +1495,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>4</v>
@@ -1515,9 +1518,9 @@
       <c r="G68" s="7"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>4</v>
@@ -1529,18 +1532,18 @@
       <c r="G69" s="7"/>
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -1548,7 +1551,7 @@
         <v>4</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7">
@@ -1558,9 +1561,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -1568,7 +1571,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7">
@@ -1578,18 +1581,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>4</v>
@@ -1601,9 +1604,9 @@
       <c r="G74" s="7"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>4</v>
@@ -1615,18 +1618,18 @@
       <c r="G75" s="7"/>
       <c r="H75" s="5"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -1634,7 +1637,7 @@
         <v>4</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7">
@@ -1655,24 +1658,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Création de la classe Salle et de son test + Modification des paramètres
- Création de la classe Salle.class.php
- Création de la classe Salle.test.php
- Modification de parametres.localhost.php
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="7125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -647,10 +647,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +665,7 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -676,7 +676,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -685,7 +685,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -696,7 +696,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -722,12 +722,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -747,12 +747,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -772,12 +772,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -797,12 +797,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -816,12 +816,12 @@
       <c r="G17" s="7"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -841,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -861,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -875,7 +875,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -889,7 +889,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -923,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -943,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -957,7 +957,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -971,7 +971,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -985,7 +985,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1057,7 +1057,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1147,7 +1147,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>17</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1209,7 +1209,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1223,7 +1223,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="G48" s="7"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -1246,7 +1246,7 @@
       <c r="G49" s="9"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="G50" s="7"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -1283,7 +1283,7 @@
       <c r="G52" s="9"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="G53" s="7"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -1320,7 +1320,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -1369,7 +1369,7 @@
       <c r="G58" s="9"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -1418,7 +1418,7 @@
       <c r="G61" s="9"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -1455,7 +1455,7 @@
       <c r="G64" s="9"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -1504,7 +1504,7 @@
       <c r="G67" s="9"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1518,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="G69" s="7"/>
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -1541,7 +1541,7 @@
       <c r="G70" s="9"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>61</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>62</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -1590,7 +1590,7 @@
       <c r="G73" s="9"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -1604,7 +1604,7 @@
       <c r="G74" s="7"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -1618,7 +1618,7 @@
       <c r="G75" s="7"/>
       <c r="H75" s="5"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
@@ -1627,7 +1627,7 @@
       <c r="G76" s="9"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Modification de la liste des taches.
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
   <si>
     <t>A faire</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve">     Développement et test CtrlTelechargerApk</t>
+  </si>
+  <si>
+    <t>Killian</t>
   </si>
 </sst>
 </file>
@@ -650,7 +653,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,15 +809,21 @@
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="7">
+        <v>42640</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">

</xml_diff>

<commit_message>
Ajout de "DemanderMdp" + Modif page index
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="67">
   <si>
     <t>A faire</t>
   </si>
@@ -652,8 +652,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,13 +1517,17 @@
       <c r="A68" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="7"/>
+      <c r="E68" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F68" s="7">
+        <v>42640</v>
+      </c>
       <c r="G68" s="7"/>
       <c r="H68" s="5"/>
     </row>
@@ -1531,13 +1535,17 @@
       <c r="A69" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="7"/>
+      <c r="E69" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F69" s="7">
+        <v>42640</v>
+      </c>
       <c r="G69" s="7"/>
       <c r="H69" s="5"/>
     </row>

</xml_diff>

<commit_message>
Fin de DemanderMdp + création de méthodes
- Finition de la vue DemanderMdp et de son contrôleur
- Méthodes : getUtilisateur et modifierMdpUser
- Mise à jour de la liste des taches
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="8775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Erwann</t>
+  </si>
+  <si>
+    <t>Tony</t>
   </si>
 </sst>
 </file>
@@ -655,20 +658,20 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="56.875" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.75" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -1111,28 +1114,40 @@
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="7">
+        <v>42641</v>
+      </c>
+      <c r="G36" s="7">
+        <v>42641</v>
+      </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
+      <c r="D37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="7">
+        <v>42641</v>
+      </c>
+      <c r="G37" s="7">
+        <v>42641</v>
+      </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1266,12 +1281,14 @@
       <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="5"/>
@@ -1280,12 +1297,14 @@
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
@@ -1438,13 +1457,17 @@
       <c r="A62" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F62" s="7">
+        <v>42640</v>
+      </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
@@ -1452,13 +1475,17 @@
       <c r="A63" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="E63" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F63" s="7">
+        <v>42640</v>
+      </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
@@ -1524,28 +1551,40 @@
       <c r="A68" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B68" s="5"/>
       <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
+      <c r="D68" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F68" s="7">
+        <v>42641</v>
+      </c>
+      <c r="G68" s="7">
+        <v>42641</v>
+      </c>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B69" s="5"/>
       <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
+      <c r="D69" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F69" s="7">
+        <v>42641</v>
+      </c>
+      <c r="G69" s="7">
+        <v>42641</v>
+      </c>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modification liste des tâches
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="7410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -658,20 +658,20 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.875" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -823,7 +823,9 @@
       <c r="E17" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>42640</v>
+      </c>
       <c r="G17" s="7">
         <v>42640</v>
       </c>
@@ -1289,7 +1291,9 @@
       <c r="E50" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="7"/>
+      <c r="F50" s="7">
+        <v>42640</v>
+      </c>
       <c r="G50" s="7"/>
       <c r="H50" s="5"/>
     </row>
@@ -1305,7 +1309,9 @@
       <c r="E51" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F51" s="5"/>
+      <c r="F51" s="7">
+        <v>42640</v>
+      </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
@@ -1560,7 +1566,7 @@
         <v>66</v>
       </c>
       <c r="F68" s="7">
-        <v>42641</v>
+        <v>42640</v>
       </c>
       <c r="G68" s="7">
         <v>42641</v>
@@ -1580,7 +1586,7 @@
         <v>66</v>
       </c>
       <c r="F69" s="7">
-        <v>42641</v>
+        <v>42640</v>
       </c>
       <c r="G69" s="7">
         <v>42641</v>

</xml_diff>

<commit_message>
Nouvelle affectation sur la liste des taches
Affectation de Erwann à :
- annulerReservation
- CtrlAnnulerReservation
- VueAnnulerReservation
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="8640"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -391,9 +391,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +410,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -724,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,15 +741,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
@@ -761,15 +761,15 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -878,24 +878,24 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="15" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="15">
         <v>42640</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="15">
         <v>42640</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -945,18 +945,22 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="5"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="18">
+        <v>42647</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1127,22 +1131,23 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18" t="s">
+      <c r="B33" s="17"/>
+      <c r="D33" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="19">
-        <v>42640</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="18"/>
+      <c r="F33" s="18">
+        <v>42647</v>
+      </c>
+      <c r="G33" s="18">
+        <v>42647</v>
+      </c>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1179,44 +1184,44 @@
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="15" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="15">
         <v>42641</v>
       </c>
-      <c r="G36" s="16">
+      <c r="G36" s="15">
         <v>42641</v>
       </c>
-      <c r="H36" s="15"/>
+      <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="15" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="15">
         <v>42641</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="15">
         <v>42641</v>
       </c>
-      <c r="H37" s="15"/>
+      <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1309,32 +1314,40 @@
       <c r="H45" s="5"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="5"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="18">
+        <v>42647</v>
+      </c>
+      <c r="G47" s="18"/>
+      <c r="H47" s="17"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="5"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="18">
+        <v>42647</v>
+      </c>
+      <c r="G48" s="18"/>
+      <c r="H48" s="17"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -1346,40 +1359,40 @@
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12" t="s">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F50" s="12">
         <v>42640</v>
       </c>
-      <c r="G50" s="13"/>
-      <c r="H50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="11"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12" t="s">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F51" s="13">
+      <c r="F51" s="12">
         <v>42640</v>
       </c>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
@@ -1526,40 +1539,44 @@
       <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18" t="s">
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F62" s="19">
-        <v>42640</v>
-      </c>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
+      <c r="F62" s="18">
+        <v>42647</v>
+      </c>
+      <c r="G62" s="18">
+        <v>42647</v>
+      </c>
+      <c r="H62" s="17"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18" t="s">
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F63" s="19">
-        <v>42640</v>
-      </c>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
+      <c r="F63" s="18">
+        <v>42647</v>
+      </c>
+      <c r="G63" s="18">
+        <v>42647</v>
+      </c>
+      <c r="H63" s="17"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
@@ -1620,44 +1637,44 @@
       <c r="H67" s="8"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E68" s="15" t="s">
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F68" s="16">
+      <c r="F68" s="15">
         <v>42640</v>
       </c>
-      <c r="G68" s="16">
+      <c r="G68" s="15">
         <v>42641</v>
       </c>
-      <c r="H68" s="15"/>
+      <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E69" s="15" t="s">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F69" s="16">
+      <c r="F69" s="15">
         <v>42640</v>
       </c>
-      <c r="G69" s="16">
+      <c r="G69" s="15">
         <v>42641</v>
       </c>
-      <c r="H69" s="15"/>
+      <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>

</xml_diff>

<commit_message>
Modification de la liste des tâches
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="8640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -325,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +335,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -413,6 +431,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -724,8 +751,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,9 +780,15 @@
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>68</v>
+      </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>

</xml_diff>

<commit_message>
Modification de la DAO et SupprimerUtilisateur et la liste des taches
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M23"/>
+  <oleSize ref="A15:D49"/>
 </workbook>
 </file>
 
@@ -808,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,20 +1125,22 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="12">
+        <v>42654</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">

</xml_diff>

<commit_message>
Modification du contrôleur SupprimerUtilisateur et la liste des taches.
- Amélioration et fin de la page de suppression de l'utilisateur
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21345" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="70">
   <si>
     <t>A faire</t>
   </si>
@@ -224,13 +224,16 @@
   </si>
   <si>
     <t>Tony</t>
+  </si>
+  <si>
+    <t>11/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +323,21 @@
     <font>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -495,10 +513,17 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,8 +833,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,33 +1064,39 @@
         <v>24</v>
       </c>
       <c r="B22" s="17"/>
-      <c r="C22" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="E22" s="17" t="s">
         <v>67</v>
       </c>
       <c r="F22" s="18">
         <v>42647</v>
       </c>
-      <c r="G22" s="18"/>
+      <c r="G22" s="18">
+        <v>42654</v>
+      </c>
       <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>4</v>
-      </c>
+      <c r="B23" s="14"/>
       <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
+      <c r="D23" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="E23" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="F23" s="15">
+        <v>42654</v>
+      </c>
+      <c r="G23" s="15">
+        <v>42654</v>
+      </c>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1129,50 +1160,60 @@
         <v>30</v>
       </c>
       <c r="B27" s="11"/>
-      <c r="C27" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="E27" s="11" t="s">
         <v>68</v>
       </c>
       <c r="F27" s="12">
         <v>42654</v>
       </c>
-      <c r="G27" s="11"/>
+      <c r="G27" s="12">
+        <v>42654</v>
+      </c>
       <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="31">
+        <v>42654</v>
+      </c>
+      <c r="G28" s="31">
+        <v>42654</v>
+      </c>
+      <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="F29" s="31">
+        <v>42654</v>
+      </c>
+      <c r="G29" s="31">
+        <v>42654</v>
+      </c>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1227,7 +1268,9 @@
         <v>13</v>
       </c>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="7">
+        <v>42614</v>
+      </c>
       <c r="H32" s="5" t="s">
         <v>4</v>
       </c>
@@ -1272,20 +1315,24 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="31">
+        <v>42654</v>
+      </c>
+      <c r="G35" s="31">
+        <v>42654</v>
+      </c>
+      <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
@@ -1331,16 +1378,20 @@
       <c r="A38" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>4</v>
-      </c>
+      <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+      <c r="D38" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="E38" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="F38" s="15">
+        <v>42654</v>
+      </c>
+      <c r="G38" s="15">
+        <v>42654</v>
+      </c>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1434,7 +1485,9 @@
       <c r="F47" s="18">
         <v>42647</v>
       </c>
-      <c r="G47" s="18"/>
+      <c r="G47" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="H47" s="17"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -1510,10 +1563,10 @@
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C53" s="23"/>
@@ -1526,10 +1579,10 @@
       <c r="H53" s="23"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="23"/>
@@ -1859,7 +1912,9 @@
       <c r="F74" s="15">
         <v>42654</v>
       </c>
-      <c r="G74" s="15"/>
+      <c r="G74" s="15">
+        <v>42654</v>
+      </c>
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit de fin de séance
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Tony</t>
-  </si>
-  <si>
-    <t>11/</t>
   </si>
 </sst>
 </file>
@@ -834,7 +831,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,9 +1482,7 @@
       <c r="F47" s="18">
         <v>42647</v>
       </c>
-      <c r="G47" s="18" t="s">
-        <v>69</v>
-      </c>
+      <c r="G47" s="18"/>
       <c r="H47" s="17"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -1505,7 +1500,9 @@
       <c r="F48" s="18">
         <v>42647</v>
       </c>
-      <c r="G48" s="18"/>
+      <c r="G48" s="18">
+        <v>42654</v>
+      </c>
       <c r="H48" s="17"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mise à jour de la DAO et des contrôleurs après la validation des pages.
- PROJET DONE
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21345" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20565" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -488,9 +488,6 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -519,6 +516,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -830,8 +830,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,25 +847,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="6"/>
@@ -873,15 +873,15 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1007,7 +1007,7 @@
       <c r="G17" s="15">
         <v>42640</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1074,7 +1074,9 @@
       <c r="G22" s="18">
         <v>42654</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
@@ -1094,23 +1096,31 @@
       <c r="G23" s="15">
         <v>42654</v>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="E24" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="F24" s="12">
+        <v>42657</v>
+      </c>
+      <c r="G24" s="12">
+        <v>42657</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1170,47 +1180,53 @@
       <c r="G27" s="12">
         <v>42654</v>
       </c>
-      <c r="H27" s="11"/>
+      <c r="H27" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="26" t="s">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="30">
         <v>42654</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="30">
         <v>42654</v>
       </c>
-      <c r="H28" s="26"/>
+      <c r="H28" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="28" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="30">
         <v>42654</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="30">
         <v>42654</v>
       </c>
-      <c r="H29" s="28"/>
+      <c r="H29" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1289,7 +1305,9 @@
       <c r="G33" s="18">
         <v>42647</v>
       </c>
-      <c r="H33" s="17"/>
+      <c r="H33" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1312,24 +1330,26 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="26" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="31">
+      <c r="F35" s="30">
         <v>42654</v>
       </c>
-      <c r="G35" s="31">
+      <c r="G35" s="30">
         <v>42654</v>
       </c>
-      <c r="H35" s="26"/>
+      <c r="H35" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
@@ -1349,7 +1369,9 @@
       <c r="G36" s="15">
         <v>42641</v>
       </c>
-      <c r="H36" s="14"/>
+      <c r="H36" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -1369,7 +1391,9 @@
       <c r="G37" s="15">
         <v>42641</v>
       </c>
-      <c r="H37" s="14"/>
+      <c r="H37" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
@@ -1389,7 +1413,9 @@
       <c r="G38" s="15">
         <v>42654</v>
       </c>
-      <c r="H38" s="14"/>
+      <c r="H38" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1399,11 +1425,21 @@
         <v>4</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="5"/>
+      <c r="D39" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="15">
+        <v>42657</v>
+      </c>
+      <c r="G39" s="15">
+        <v>42657</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1456,44 +1492,54 @@
         <v>44</v>
       </c>
       <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="E45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="5"/>
+      <c r="F45" s="7">
+        <v>42640</v>
+      </c>
+      <c r="G45" s="7">
+        <v>42657</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="17"/>
-      <c r="C47" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="E47" s="17" t="s">
         <v>67</v>
       </c>
       <c r="F47" s="18">
         <v>42647</v>
       </c>
-      <c r="G47" s="18"/>
-      <c r="H47" s="17"/>
+      <c r="G47" s="18">
+        <v>42657</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="17"/>
-      <c r="C48" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="E48" s="17" t="s">
         <v>67</v>
       </c>
@@ -1503,7 +1549,9 @@
       <c r="G48" s="18">
         <v>42654</v>
       </c>
-      <c r="H48" s="17"/>
+      <c r="H48" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -1519,36 +1567,44 @@
         <v>47</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="E50" s="11" t="s">
         <v>68</v>
       </c>
       <c r="F50" s="12">
         <v>42640</v>
       </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="11"/>
+      <c r="G50" s="12">
+        <v>42640</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B51" s="11"/>
-      <c r="C51" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="E51" s="11" t="s">
         <v>68</v>
       </c>
       <c r="F51" s="12">
         <v>42640</v>
       </c>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+      <c r="G51" s="12">
+        <v>42640</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
@@ -1560,36 +1616,48 @@
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23" t="s">
+      <c r="B53" s="28"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="23"/>
+      <c r="F53" s="23">
+        <v>42657</v>
+      </c>
+      <c r="G53" s="23">
+        <v>42657</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23" t="s">
+      <c r="B54" s="28"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
+      <c r="F54" s="23">
+        <v>42657</v>
+      </c>
+      <c r="G54" s="23">
+        <v>42657</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
@@ -1716,7 +1784,9 @@
       <c r="G62" s="18">
         <v>42647</v>
       </c>
-      <c r="H62" s="17"/>
+      <c r="H62" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
@@ -1736,7 +1806,9 @@
       <c r="G63" s="18">
         <v>42647</v>
       </c>
-      <c r="H63" s="17"/>
+      <c r="H63" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
@@ -1814,7 +1886,9 @@
       <c r="G68" s="15">
         <v>42641</v>
       </c>
-      <c r="H68" s="14"/>
+      <c r="H68" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
@@ -1834,7 +1908,9 @@
       <c r="G69" s="15">
         <v>42641</v>
       </c>
-      <c r="H69" s="14"/>
+      <c r="H69" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
@@ -1899,10 +1975,10 @@
         <v>63</v>
       </c>
       <c r="B74" s="14"/>
-      <c r="C74" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="E74" s="14" t="s">
         <v>66</v>
       </c>
@@ -1912,25 +1988,31 @@
       <c r="G74" s="15">
         <v>42654</v>
       </c>
-      <c r="H74" s="14"/>
+      <c r="H74" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B75" s="14"/>
-      <c r="C75" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="E75" s="14" t="s">
         <v>66</v>
       </c>
       <c r="F75" s="15">
         <v>42654</v>
       </c>
-      <c r="G75" s="15"/>
-      <c r="H75" s="14"/>
+      <c r="G75" s="15">
+        <v>42654</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>

</xml_diff>